<commit_message>
Replace UK regions and correct map instructors
</commit_message>
<xml_diff>
--- a/lib/UK-regions-airports.xlsx
+++ b/lib/UK-regions-airports.xlsx
@@ -11,14 +11,14 @@
     <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UK-regions-airports'!$A$1:$C$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UK-regions-airports'!$A$1:$C$75</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="166">
   <si>
     <t>Airport_code</t>
   </si>
@@ -29,18 +29,9 @@
     <t>UK_region</t>
   </si>
   <si>
-    <t>EAST MIDLANDS</t>
-  </si>
-  <si>
     <t>East Midlands Airport</t>
   </si>
   <si>
-    <t>Leicester Airport</t>
-  </si>
-  <si>
-    <t>EAST OF ENGLAND</t>
-  </si>
-  <si>
     <t>Cambridge International Airport</t>
   </si>
   <si>
@@ -59,9 +50,6 @@
     <t>London Stansted Airport</t>
   </si>
   <si>
-    <t>LONDON</t>
-  </si>
-  <si>
     <t>London Biggin Hill Airport</t>
   </si>
   <si>
@@ -71,33 +59,6 @@
     <t>London City Airport</t>
   </si>
   <si>
-    <t>NORTH EAST</t>
-  </si>
-  <si>
-    <t>NORTH WEST</t>
-  </si>
-  <si>
-    <t>YORKSHIRE AND THE HUMBER</t>
-  </si>
-  <si>
-    <t>WEST MIDLANDS</t>
-  </si>
-  <si>
-    <t>SOUTH EAST</t>
-  </si>
-  <si>
-    <t>SOUTH WEST</t>
-  </si>
-  <si>
-    <t>WALES</t>
-  </si>
-  <si>
-    <t>SCOTLAND</t>
-  </si>
-  <si>
-    <t>NORTHERN IRELAND</t>
-  </si>
-  <si>
     <t>Durham Tees Valley Airport</t>
   </si>
   <si>
@@ -107,9 +68,6 @@
     <t>It contains info on UK airports and their corresponding UK region.</t>
   </si>
   <si>
-    <t>Data in sheet 'UK-regions-airports' was extracted on 2017-10-16 from https://en.wikipedia.org/wiki/List_of_airports_in_the_United_Kingdom_and_the_British_Crown_Dependencies.</t>
-  </si>
-  <si>
     <t>Barrow/Walney Island Airport</t>
   </si>
   <si>
@@ -182,346 +140,382 @@
     <t>Leeds Bradford International Airport</t>
   </si>
   <si>
+    <t>Aberdeen International Airport</t>
+  </si>
+  <si>
+    <t>Oban Airport</t>
+  </si>
+  <si>
+    <t>Benbecula Airport</t>
+  </si>
+  <si>
+    <t>Barra Airport</t>
+  </si>
+  <si>
+    <t>Campbeltown Airport</t>
+  </si>
+  <si>
+    <t>Coll Airport</t>
+  </si>
+  <si>
+    <t>Colonsay Airport</t>
+  </si>
+  <si>
+    <t>North Ronaldsay Airport</t>
+  </si>
+  <si>
+    <t>Inverness Airport</t>
+  </si>
+  <si>
+    <t>Scatsta Airport</t>
+  </si>
+  <si>
+    <t>Dundee Airport</t>
+  </si>
+  <si>
+    <t>Sumburgh Airport</t>
+  </si>
+  <si>
+    <t>Eday Airport</t>
+  </si>
+  <si>
+    <t>Edinburgh Airport</t>
+  </si>
+  <si>
+    <t>Islay Airport</t>
+  </si>
+  <si>
+    <t>Sanday Airport</t>
+  </si>
+  <si>
+    <t>Papa Westray Airport</t>
+  </si>
+  <si>
+    <t>Glasgow Prestwick Airport</t>
+  </si>
+  <si>
+    <t>Glasgow International Airport</t>
+  </si>
+  <si>
+    <t>Kirkwall Airport</t>
+  </si>
+  <si>
+    <t>Perth Airport</t>
+  </si>
+  <si>
+    <t>Stornoway Airport</t>
+  </si>
+  <si>
+    <t>Broadford Airfield</t>
+  </si>
+  <si>
+    <t>Stronsay Airport</t>
+  </si>
+  <si>
+    <t>Tingwall Airport</t>
+  </si>
+  <si>
+    <t>Tiree Airport</t>
+  </si>
+  <si>
+    <t>Westray Airport</t>
+  </si>
+  <si>
+    <t>Whalsay Airport</t>
+  </si>
+  <si>
+    <t>Wick Airport</t>
+  </si>
+  <si>
+    <t>Haverfordwest Aerodrome</t>
+  </si>
+  <si>
+    <t>Chester Hawarden Airport</t>
+  </si>
+  <si>
+    <t>Anglesey Airport</t>
+  </si>
+  <si>
+    <t>Swansea Airport</t>
+  </si>
+  <si>
+    <t>Cardiff Airport</t>
+  </si>
+  <si>
+    <t>MME</t>
+  </si>
+  <si>
+    <t>NCL</t>
+  </si>
+  <si>
+    <t>BWF</t>
+  </si>
+  <si>
+    <t>CAX</t>
+  </si>
+  <si>
+    <t>LPL</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>HUY</t>
+  </si>
+  <si>
+    <t>LBA</t>
+  </si>
+  <si>
+    <t>EMA</t>
+  </si>
+  <si>
+    <t>CVT</t>
+  </si>
+  <si>
+    <t>BHX</t>
+  </si>
+  <si>
+    <t>CBG</t>
+  </si>
+  <si>
+    <t>QFO</t>
+  </si>
+  <si>
+    <t>LTN</t>
+  </si>
+  <si>
+    <t>NWI</t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
+    <t>STN</t>
+  </si>
+  <si>
+    <t>BQH</t>
+  </si>
+  <si>
+    <t>LHR</t>
+  </si>
+  <si>
+    <t>LCY</t>
+  </si>
+  <si>
+    <t>LGW</t>
+  </si>
+  <si>
+    <t>SOU</t>
+  </si>
+  <si>
+    <t>ESH</t>
+  </si>
+  <si>
+    <t>QLA</t>
+  </si>
+  <si>
+    <t>LYX</t>
+  </si>
+  <si>
+    <t>KRH</t>
+  </si>
+  <si>
+    <t>QUG</t>
+  </si>
+  <si>
+    <t>BBS</t>
+  </si>
+  <si>
+    <t>GLO</t>
+  </si>
+  <si>
+    <t>EXT</t>
+  </si>
+  <si>
+    <t>BOH</t>
+  </si>
+  <si>
+    <t>NQY</t>
+  </si>
+  <si>
+    <t>LEQ</t>
+  </si>
+  <si>
+    <t>ISC</t>
+  </si>
+  <si>
+    <t>BRS</t>
+  </si>
+  <si>
+    <t>HAW</t>
+  </si>
+  <si>
+    <t>CEG</t>
+  </si>
+  <si>
+    <t>VLY</t>
+  </si>
+  <si>
+    <t>SWS</t>
+  </si>
+  <si>
+    <t>CWL</t>
+  </si>
+  <si>
+    <t>ABZ</t>
+  </si>
+  <si>
+    <t>OBN</t>
+  </si>
+  <si>
+    <t>BEB</t>
+  </si>
+  <si>
+    <t>BRR</t>
+  </si>
+  <si>
+    <t>CAL</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>CSA</t>
+  </si>
+  <si>
+    <t>NRL</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>SCS</t>
+  </si>
+  <si>
+    <t>DND</t>
+  </si>
+  <si>
+    <t>LSI</t>
+  </si>
+  <si>
+    <t>EOI</t>
+  </si>
+  <si>
+    <t>EDI</t>
+  </si>
+  <si>
+    <t>ILY</t>
+  </si>
+  <si>
+    <t>NDY</t>
+  </si>
+  <si>
+    <t>PPW</t>
+  </si>
+  <si>
+    <t>PIK</t>
+  </si>
+  <si>
+    <t>GLA</t>
+  </si>
+  <si>
+    <t>KOI</t>
+  </si>
+  <si>
+    <t>PSL</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>SKL</t>
+  </si>
+  <si>
+    <t>SOY</t>
+  </si>
+  <si>
+    <t>LWK</t>
+  </si>
+  <si>
+    <t>TRE</t>
+  </si>
+  <si>
+    <t>WRY</t>
+  </si>
+  <si>
+    <t>WHS</t>
+  </si>
+  <si>
+    <t>WIC</t>
+  </si>
+  <si>
+    <t>The list only includes public airports with and IATA code. Military and Private airports were excluded even if IATA code present, except ADX that it was added because on of the users inserted that value.</t>
+  </si>
+  <si>
+    <t>ADX</t>
+  </si>
+  <si>
+    <t>RAF Leuchars</t>
+  </si>
+  <si>
+    <t>Data in sheet 'UK-regions-airports' was extracted on 2017-10-16 from https://en.wikipedia.org/wiki/List_of_airports_in_the_United_Kingdom_and_the_British_Crown_Dependencies</t>
+  </si>
+  <si>
+    <t>North East</t>
+  </si>
+  <si>
+    <t>North West</t>
+  </si>
+  <si>
+    <t>Yorkshire and The Humber</t>
+  </si>
+  <si>
+    <t>East Midlands</t>
+  </si>
+  <si>
+    <t>West Midlands</t>
+  </si>
+  <si>
+    <t>Eastern</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>South East</t>
+  </si>
+  <si>
+    <t>South West</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
     <t>Belfast International Airport</t>
   </si>
   <si>
+    <t>BHD</t>
+  </si>
+  <si>
     <t>George Best Belfast City Airport</t>
   </si>
   <si>
+    <t>LDY</t>
+  </si>
+  <si>
     <t>City of Derry Airport</t>
   </si>
   <si>
-    <t>Aberdeen International Airport</t>
-  </si>
-  <si>
-    <t>Oban Airport</t>
-  </si>
-  <si>
-    <t>Benbecula Airport</t>
-  </si>
-  <si>
-    <t>Barra Airport</t>
-  </si>
-  <si>
-    <t>Campbeltown Airport</t>
-  </si>
-  <si>
-    <t>Coll Airport</t>
-  </si>
-  <si>
-    <t>Colonsay Airport</t>
-  </si>
-  <si>
-    <t>North Ronaldsay Airport</t>
-  </si>
-  <si>
-    <t>Inverness Airport</t>
-  </si>
-  <si>
-    <t>Scatsta Airport</t>
-  </si>
-  <si>
-    <t>Dundee Airport</t>
-  </si>
-  <si>
-    <t>Sumburgh Airport</t>
-  </si>
-  <si>
-    <t>Eday Airport</t>
-  </si>
-  <si>
-    <t>Edinburgh Airport</t>
-  </si>
-  <si>
-    <t>Islay Airport</t>
-  </si>
-  <si>
-    <t>Sanday Airport</t>
-  </si>
-  <si>
-    <t>Papa Westray Airport</t>
-  </si>
-  <si>
-    <t>Glasgow Prestwick Airport</t>
-  </si>
-  <si>
-    <t>Glasgow International Airport</t>
-  </si>
-  <si>
-    <t>Kirkwall Airport</t>
-  </si>
-  <si>
-    <t>Perth Airport</t>
-  </si>
-  <si>
-    <t>Stornoway Airport</t>
-  </si>
-  <si>
-    <t>Broadford Airfield</t>
-  </si>
-  <si>
-    <t>Stronsay Airport</t>
-  </si>
-  <si>
-    <t>Tingwall Airport</t>
-  </si>
-  <si>
-    <t>Tiree Airport</t>
-  </si>
-  <si>
-    <t>Westray Airport</t>
-  </si>
-  <si>
-    <t>Whalsay Airport</t>
-  </si>
-  <si>
-    <t>Wick Airport</t>
-  </si>
-  <si>
-    <t>Haverfordwest Aerodrome</t>
-  </si>
-  <si>
-    <t>Chester Hawarden Airport</t>
-  </si>
-  <si>
-    <t>Anglesey Airport</t>
-  </si>
-  <si>
-    <t>Swansea Airport</t>
-  </si>
-  <si>
-    <t>Cardiff Airport</t>
-  </si>
-  <si>
-    <t>MME</t>
-  </si>
-  <si>
-    <t>NCL</t>
-  </si>
-  <si>
-    <t>BWF</t>
-  </si>
-  <si>
-    <t>CAX</t>
-  </si>
-  <si>
-    <t>LPL</t>
-  </si>
-  <si>
-    <t>MAN</t>
-  </si>
-  <si>
-    <t>DSA</t>
-  </si>
-  <si>
-    <t>HUY</t>
-  </si>
-  <si>
-    <t>LBA</t>
-  </si>
-  <si>
-    <t>EMA</t>
-  </si>
-  <si>
-    <t>LRC</t>
-  </si>
-  <si>
-    <t>CVT</t>
-  </si>
-  <si>
-    <t>BHX</t>
-  </si>
-  <si>
-    <t>CBG</t>
-  </si>
-  <si>
-    <t>QFO</t>
-  </si>
-  <si>
-    <t>LTN</t>
-  </si>
-  <si>
-    <t>NWI</t>
-  </si>
-  <si>
-    <t>SEN</t>
-  </si>
-  <si>
-    <t>STN</t>
-  </si>
-  <si>
-    <t>BQH</t>
-  </si>
-  <si>
-    <t>LHR</t>
-  </si>
-  <si>
-    <t>LCY</t>
-  </si>
-  <si>
-    <t>LGW</t>
-  </si>
-  <si>
-    <t>SOU</t>
-  </si>
-  <si>
-    <t>ESH</t>
-  </si>
-  <si>
-    <t>QLA</t>
-  </si>
-  <si>
-    <t>LYX</t>
-  </si>
-  <si>
-    <t>KRH</t>
-  </si>
-  <si>
-    <t>QUG</t>
-  </si>
-  <si>
-    <t>BBS</t>
-  </si>
-  <si>
-    <t>GLO</t>
-  </si>
-  <si>
-    <t>EXT</t>
-  </si>
-  <si>
-    <t>BOH</t>
-  </si>
-  <si>
-    <t>NQY</t>
-  </si>
-  <si>
-    <t>LEQ</t>
-  </si>
-  <si>
-    <t>ISC</t>
-  </si>
-  <si>
-    <t>BRS</t>
-  </si>
-  <si>
-    <t>HAW</t>
-  </si>
-  <si>
-    <t>CEG</t>
-  </si>
-  <si>
-    <t>VLY</t>
-  </si>
-  <si>
-    <t>SWS</t>
-  </si>
-  <si>
-    <t>CWL</t>
-  </si>
-  <si>
-    <t>ABZ</t>
-  </si>
-  <si>
-    <t>OBN</t>
-  </si>
-  <si>
-    <t>BEB</t>
-  </si>
-  <si>
-    <t>BRR</t>
-  </si>
-  <si>
-    <t>CAL</t>
-  </si>
-  <si>
-    <t>COL</t>
-  </si>
-  <si>
-    <t>CSA</t>
-  </si>
-  <si>
-    <t>NRL</t>
-  </si>
-  <si>
-    <t>INV</t>
-  </si>
-  <si>
-    <t>SCS</t>
-  </si>
-  <si>
-    <t>DND</t>
-  </si>
-  <si>
-    <t>LSI</t>
-  </si>
-  <si>
-    <t>EOI</t>
-  </si>
-  <si>
-    <t>EDI</t>
-  </si>
-  <si>
-    <t>ILY</t>
-  </si>
-  <si>
-    <t>NDY</t>
-  </si>
-  <si>
-    <t>PPW</t>
-  </si>
-  <si>
-    <t>PIK</t>
-  </si>
-  <si>
-    <t>GLA</t>
-  </si>
-  <si>
-    <t>KOI</t>
-  </si>
-  <si>
-    <t>PSL</t>
-  </si>
-  <si>
-    <t>SYY</t>
-  </si>
-  <si>
-    <t>SKL</t>
-  </si>
-  <si>
-    <t>SOY</t>
-  </si>
-  <si>
-    <t>LWK</t>
-  </si>
-  <si>
-    <t>TRE</t>
-  </si>
-  <si>
-    <t>WRY</t>
-  </si>
-  <si>
-    <t>WHS</t>
-  </si>
-  <si>
-    <t>WIC</t>
-  </si>
-  <si>
-    <t>BFS</t>
-  </si>
-  <si>
-    <t>BHD</t>
-  </si>
-  <si>
-    <t>LDY</t>
-  </si>
-  <si>
-    <t>The list only includes public airports with and IATA code. Military and Private airports were excluded even if IATA code present, except ADX that it was added because on of the users inserted that value.</t>
-  </si>
-  <si>
-    <t>ADX</t>
-  </si>
-  <si>
-    <t>RAF Leuchars</t>
+    <t>Northern Ireland</t>
   </si>
 </sst>
 </file>
@@ -860,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,805 +880,805 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C69" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="C73" t="s">
-        <v>24</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>161</v>
+      </c>
+      <c r="B74" t="s">
         <v>162</v>
       </c>
-      <c r="B74" t="s">
-        <v>54</v>
-      </c>
       <c r="C74" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1692,25 +1686,14 @@
         <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>164</v>
-      </c>
-      <c r="B76" t="s">
-        <v>56</v>
-      </c>
-      <c r="C76" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C76"/>
+  <autoFilter ref="A1:C75"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1719,25 +1702,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>